<commit_message>
table 24 riset group aktif laman admin
</commit_message>
<xml_diff>
--- a/public/template/rida/mboh/table_18_researchgroupaktif.xlsx
+++ b/public/template/rida/mboh/table_18_researchgroupaktif.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univ11maret-my.sharepoint.com/personal/muhasyai_365_uns_ac_id/Documents/~ Muhammad Syaifudin/Kerjaan Kantor/~ BIRO RISET DAN PENGABDIAN MASYARAKAT/RIDA/2021 02/Draft Ver.2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\iris1103\public\template\rida\mboh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{DF5A41F8-446A-4542-A430-DA2F00BBAF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F7D530C-C80B-407C-B066-EDA3A229C5B9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6A9AE4-4936-4EC6-8D81-334D91A6025A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{4E0C8446-EE1A-4CC4-87F1-B695B5DF7E8C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{4E0C8446-EE1A-4CC4-87F1-B695B5DF7E8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,13 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -562,15 +569,15 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.59765625" customWidth="1"/>
+    <col min="1" max="1" width="41.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>19</v>
       </c>
@@ -580,7 +587,7 @@
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
     </row>
-    <row r="2" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>17</v>
       </c>
@@ -590,7 +597,7 @@
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
     </row>
-    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
@@ -602,7 +609,7 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
       <c r="B5" s="6">
         <v>2017</v>
@@ -620,7 +627,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -640,7 +647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -660,7 +667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -680,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -700,7 +707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -720,7 +727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -740,7 +747,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -760,7 +767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -780,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -800,7 +807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -820,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -840,7 +847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -860,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -880,7 +887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -900,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>16</v>
       </c>
@@ -925,7 +932,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" ht="10.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -933,7 +940,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>

</xml_diff>